<commit_message>
Updated mapping and progress .xlsx
</commit_message>
<xml_diff>
--- a/Mappings/PlannedCareActivity - STU3.xlsx
+++ b/Mappings/PlannedCareActivity - STU3.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="182">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -557,13 +557,19 @@
   </si>
   <si>
     <t>Contact</t>
+  </si>
+  <si>
+    <t>OverdrachtGeplandeZorgActiviteit MedicalAid</t>
+  </si>
+  <si>
+    <t>DeviceRequest.occurrence.end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -603,8 +609,20 @@
       <color rgb="FFFF0000"/>
       <name val="Open sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,6 +651,16 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -814,11 +842,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -975,27 +1005,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1005,14 +1042,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1313,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1334,15 +1368,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1355,16 +1389,16 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="71"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="74"/>
       <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1641,19 +1675,19 @@
       <c r="J14" s="37"/>
       <c r="K14" s="38"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1664,24 +1698,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" s="3"/>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="71"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="74"/>
       <c r="J18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -1703,8 +1737,9 @@
         <v>93</v>
       </c>
       <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="66"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="12">
         <v>2</v>
       </c>
@@ -1726,8 +1761,9 @@
         <v>94</v>
       </c>
       <c r="K20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="38.25">
+      <c r="M20" s="66"/>
+    </row>
+    <row r="21" spans="1:13" ht="38.25">
       <c r="A21" s="12">
         <v>3</v>
       </c>
@@ -1751,8 +1787,9 @@
       <c r="K21" s="39" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="66"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="12">
         <v>4</v>
       </c>
@@ -1773,8 +1810,9 @@
       <c r="K22" s="35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="66"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="20">
         <v>5</v>
       </c>
@@ -1790,8 +1828,9 @@
       <c r="I23" s="20"/>
       <c r="J23" s="40"/>
       <c r="K23" s="34"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="66"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="20">
         <v>6</v>
       </c>
@@ -1816,8 +1855,9 @@
       <c r="L24" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="66"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="12">
         <v>7</v>
       </c>
@@ -1842,8 +1882,9 @@
       <c r="L25" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="66"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -1868,8 +1909,9 @@
       <c r="L26" s="31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="66"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="20">
         <v>9</v>
       </c>
@@ -1894,8 +1936,9 @@
       <c r="L27" s="31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="66"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="20">
         <v>10</v>
       </c>
@@ -1920,8 +1963,9 @@
       <c r="L28" s="31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="66"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="20"/>
       <c r="B29" s="42"/>
       <c r="C29" s="31"/>
@@ -1944,8 +1988,9 @@
       <c r="L29" s="31" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="66"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="20"/>
       <c r="B30" s="42"/>
       <c r="C30" s="31"/>
@@ -1968,8 +2013,9 @@
       <c r="L30" s="31" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="66"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="12">
         <v>11</v>
       </c>
@@ -1994,8 +2040,9 @@
       <c r="L31" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="25.5">
+      <c r="M31" s="66"/>
+    </row>
+    <row r="32" spans="1:13" ht="25.5">
       <c r="A32" s="12">
         <v>12</v>
       </c>
@@ -2022,8 +2069,9 @@
       <c r="L32" s="31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="66"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="20">
         <v>13</v>
       </c>
@@ -2050,8 +2098,9 @@
       <c r="L33" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="66"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="30">
         <v>14</v>
       </c>
@@ -2076,20 +2125,21 @@
       <c r="L34" s="33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M34" s="66"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
       <c r="I38" s="1" t="s">
         <v>2</v>
       </c>
@@ -2100,24 +2150,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13">
       <c r="A39" s="3"/>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="70"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
       <c r="J39" s="32" t="s">
         <v>132</v>
       </c>
       <c r="K39" s="32"/>
     </row>
-    <row r="40" spans="1:12" ht="25.5">
+    <row r="40" spans="1:13" ht="25.5">
       <c r="A40" s="5">
         <v>1</v>
       </c>
@@ -2139,8 +2189,9 @@
         <v>137</v>
       </c>
       <c r="K40" s="34"/>
-    </row>
-    <row r="41" spans="1:12" ht="25.5">
+      <c r="M40" s="66"/>
+    </row>
+    <row r="41" spans="1:13" ht="25.5">
       <c r="A41" s="12">
         <v>2</v>
       </c>
@@ -2162,8 +2213,9 @@
         <v>137</v>
       </c>
       <c r="K41" s="18"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="66"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="12">
         <v>3</v>
       </c>
@@ -2185,8 +2237,9 @@
       <c r="K42" s="39" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" s="66"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="12">
         <v>4</v>
       </c>
@@ -2207,8 +2260,9 @@
       <c r="K43" s="35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" s="66"/>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="20">
         <v>5</v>
       </c>
@@ -2227,8 +2281,9 @@
       <c r="L44" s="14" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" s="66"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="20">
         <v>6</v>
       </c>
@@ -2249,8 +2304,9 @@
         <v>136</v>
       </c>
       <c r="K45" s="53"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="66"/>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="21">
         <v>7</v>
       </c>
@@ -2264,32 +2320,33 @@
       <c r="I46" s="63"/>
       <c r="J46" s="62"/>
       <c r="K46" s="62"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="66"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="H47" s="42"/>
       <c r="I47" s="46"/>
       <c r="J47" s="42"/>
       <c r="K47" s="42"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:13">
       <c r="H48" s="42"/>
       <c r="I48" s="46"/>
       <c r="J48" s="42"/>
       <c r="K48" s="42"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="64" t="s">
+      <c r="B49" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73"/>
+      <c r="G49" s="73"/>
+      <c r="H49" s="73"/>
       <c r="I49" s="1" t="s">
         <v>2</v>
       </c>
@@ -2300,24 +2357,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:13">
       <c r="A50" s="3"/>
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="70"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="71"/>
       <c r="J50" s="32" t="s">
         <v>78</v>
       </c>
       <c r="K50" s="32"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:13">
       <c r="A51" s="5">
         <v>1</v>
       </c>
@@ -2339,8 +2396,9 @@
         <v>148</v>
       </c>
       <c r="K51" s="34"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="66"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="12">
         <v>2</v>
       </c>
@@ -2362,8 +2420,9 @@
         <v>149</v>
       </c>
       <c r="K52" s="18"/>
-    </row>
-    <row r="53" spans="1:12" ht="51">
+      <c r="M52" s="66"/>
+    </row>
+    <row r="53" spans="1:13" ht="51">
       <c r="A53" s="12">
         <v>3</v>
       </c>
@@ -2387,8 +2446,9 @@
       <c r="K53" s="39" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" s="66"/>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="12">
         <v>4</v>
       </c>
@@ -2409,8 +2469,9 @@
       <c r="K54" s="35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" s="66"/>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="20">
         <v>5</v>
       </c>
@@ -2426,8 +2487,9 @@
       <c r="I55" s="56"/>
       <c r="J55" s="40"/>
       <c r="K55" s="34"/>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="66"/>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="20">
         <v>6</v>
       </c>
@@ -2441,15 +2503,16 @@
         <v>140</v>
       </c>
       <c r="H56" s="41"/>
-      <c r="I56" s="74" t="s">
+      <c r="I56" s="64" t="s">
         <v>7</v>
       </c>
       <c r="J56" s="41" t="s">
         <v>175</v>
       </c>
       <c r="K56" s="53"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" s="77"/>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="12">
         <v>7</v>
       </c>
@@ -2462,15 +2525,16 @@
         <v>142</v>
       </c>
       <c r="H57" s="41"/>
-      <c r="I57" s="74" t="s">
+      <c r="I57" s="64" t="s">
         <v>8</v>
       </c>
       <c r="J57" s="41" t="s">
         <v>174</v>
       </c>
       <c r="K57" s="53"/>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" s="66"/>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="12">
         <v>8</v>
       </c>
@@ -2478,11 +2542,12 @@
         <v>143</v>
       </c>
       <c r="H58" s="41"/>
-      <c r="I58" s="74"/>
+      <c r="I58" s="64"/>
       <c r="J58" s="41"/>
       <c r="K58" s="53"/>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" s="66"/>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="12">
         <v>9</v>
       </c>
@@ -2493,15 +2558,16 @@
         <v>145</v>
       </c>
       <c r="H59" s="41"/>
-      <c r="I59" s="74" t="s">
+      <c r="I59" s="64" t="s">
         <v>8</v>
       </c>
       <c r="J59" s="41" t="s">
         <v>172</v>
       </c>
       <c r="K59" s="53"/>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="66"/>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="20">
         <v>10</v>
       </c>
@@ -2512,7 +2578,7 @@
         <v>5</v>
       </c>
       <c r="H60" s="41"/>
-      <c r="I60" s="74" t="s">
+      <c r="I60" s="64" t="s">
         <v>8</v>
       </c>
       <c r="J60" s="41" t="s">
@@ -2522,8 +2588,9 @@
       <c r="L60" s="33" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60" s="66"/>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="30">
         <v>11</v>
       </c>
@@ -2538,27 +2605,28 @@
         <v>147</v>
       </c>
       <c r="H61" s="45"/>
-      <c r="I61" s="75" t="s">
+      <c r="I61" s="65" t="s">
         <v>22</v>
       </c>
       <c r="J61" s="45" t="s">
         <v>173</v>
       </c>
       <c r="K61" s="62"/>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M61" s="66"/>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="64" t="s">
+      <c r="B64" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="64"/>
-      <c r="D64" s="64"/>
-      <c r="E64" s="65"/>
-      <c r="F64" s="65"/>
-      <c r="G64" s="65"/>
-      <c r="H64" s="65"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
       <c r="I64" s="1" t="s">
         <v>2</v>
       </c>
@@ -2569,24 +2637,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:13">
       <c r="A65" s="3"/>
-      <c r="B65" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="67"/>
-      <c r="D65" s="67"/>
-      <c r="E65" s="67"/>
-      <c r="F65" s="68"/>
-      <c r="G65" s="68"/>
-      <c r="H65" s="69"/>
-      <c r="I65" s="70"/>
+      <c r="B65" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="71"/>
       <c r="J65" s="32" t="s">
         <v>176</v>
       </c>
       <c r="K65" s="32"/>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:13">
       <c r="A66" s="5">
         <v>1</v>
       </c>
@@ -2608,8 +2676,9 @@
         <v>177</v>
       </c>
       <c r="K66" s="57"/>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66" s="66"/>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="12">
         <v>2</v>
       </c>
@@ -2628,11 +2697,12 @@
         <v>6</v>
       </c>
       <c r="J67" s="41" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="K67" s="43"/>
-    </row>
-    <row r="68" spans="1:12" ht="38.25">
+      <c r="M67" s="66"/>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="12">
         <v>3</v>
       </c>
@@ -2653,11 +2723,10 @@
       <c r="J68" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="K68" s="54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="K68" s="54"/>
+      <c r="M68" s="66"/>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="12">
         <v>4</v>
       </c>
@@ -2678,8 +2747,9 @@
       <c r="K69" s="58" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69" s="66"/>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="30">
         <v>5</v>
       </c>
@@ -2702,15 +2772,16 @@
       <c r="L70" s="33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70" s="66"/>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="20"/>
       <c r="B71" s="28"/>
       <c r="E71" s="14"/>
       <c r="F71" s="15"/>
       <c r="H71" s="42"/>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:13">
       <c r="A72" s="12"/>
       <c r="B72" s="42"/>
       <c r="C72" s="14"/>
@@ -2754,16 +2825,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="27" customFormat="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="27" t="s">
@@ -3150,11 +3221,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="27" t="s">

</xml_diff>